<commit_message>
TJLP, SELIC e CDI
</commit_message>
<xml_diff>
--- a/planilhas/cotacoes.xlsx
+++ b/planilhas/cotacoes.xlsx
@@ -15,9 +15,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -63,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -74,6 +77,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -471,6 +476,26 @@
         </is>
       </c>
       <c r="K1" s="1" t="n"/>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>TJLP</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>SELIC</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>CDI</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Situacao</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -563,7 +588,7 @@
       <c r="K3" s="4" t="n">
         <v>6.7187</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>OK 22/01/2026 16:43:47</t>
         </is>
@@ -603,7 +628,7 @@
       <c r="K4" s="4" t="n">
         <v>6.7029</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>OK 23/01/2026 16:23:25</t>
         </is>
@@ -643,7 +668,7 @@
       <c r="K5" s="4" t="n">
         <v>6.8183</v>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>OK 26/01/2026 16:10:26</t>
         </is>
@@ -677,9 +702,46 @@
       <c r="K6" s="4" t="n">
         <v>6.7386</v>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>OK 04/02/2026 14:31:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>46064</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>5.183</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>5.1836</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>6.146</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>6.1477</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>6.7076</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>6.7102</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0.0919</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N7" s="7" t="n">
+        <v>0.0551310642</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>OK 11/02/2026 16:53:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
alteracao de comportamento e atualizacoes pontuais
</commit_message>
<xml_diff>
--- a/planilhas/cotacoes.xlsx
+++ b/planilhas/cotacoes.xlsx
@@ -15,12 +15,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -66,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -77,8 +76,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -730,18 +731,49 @@
       <c r="K7" s="4" t="n">
         <v>6.7102</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="L7" s="8" t="n">
         <v>0.0919</v>
       </c>
-      <c r="M7" s="6" t="n">
+      <c r="M7" s="8" t="n">
         <v>0.15</v>
       </c>
-      <c r="N7" s="7" t="n">
+      <c r="N7" s="9" t="n">
         <v>0.0551310642</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
           <t>OK 11/02/2026 16:53:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>46065</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>5.1836</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>5.1856</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>5.2147</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>5.3947</v>
+      </c>
+      <c r="L8" s="8" t="n">
+        <v>0.0919</v>
+      </c>
+      <c r="M8" s="8" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N8" s="9" t="n">
+        <v>0.0551310642</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>OK 12/02/2026 07:55:30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
alteracoes esteticas do excel
</commit_message>
<xml_diff>
--- a/planilhas/cotacoes.xlsx
+++ b/planilhas/cotacoes.xlsx
@@ -8,7 +8,9 @@
   <sheets>
     <sheet name="Cotacoes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cotacoes'!$A$2:$O$8</definedName>
+  </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -21,7 +23,7 @@
     <numFmt numFmtId="166" formatCode="0.0000%"/>
     <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,16 +31,47 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="001F2937"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DCE6F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ECF3FB"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -61,11 +94,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="009CB6D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="009CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="009CB6D9"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="009CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="009CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="009CB6D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -80,6 +160,48 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,358 +548,399 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="46.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13.42578125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="10" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="9.42578125" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="10.5" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12.5" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.5" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="12.5" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="11.5" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="12.5" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60" customHeight="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="2" t="inlineStr">
+    <row r="1" ht="22" customHeight="1">
+      <c r="A1" s="10" t="n"/>
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Dólar Oficial 
 (Fechamento)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="10" t="n"/>
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>Dólar PTAX</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="10" t="n"/>
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>Dólar Turismo</t>
         </is>
       </c>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" s="10" t="n"/>
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>Euro PTAX</t>
         </is>
       </c>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="I1" s="10" t="n"/>
+      <c r="J1" s="10" t="inlineStr">
         <is>
           <t>CHF PTAX</t>
         </is>
       </c>
-      <c r="K1" s="1" t="n"/>
-      <c r="L1" t="inlineStr">
+      <c r="K1" s="10" t="n"/>
+      <c r="L1" s="10" t="n"/>
+      <c r="M1" s="10" t="n"/>
+      <c r="N1" s="10" t="n"/>
+      <c r="O1" s="10" t="n"/>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="E2" s="11" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
+      <c r="F2" s="11" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="G2" s="11" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
+      <c r="H2" s="11" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="I2" s="11" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
+      <c r="J2" s="11" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="K2" s="11" t="inlineStr">
+        <is>
+          <t>Venda</t>
+        </is>
+      </c>
+      <c r="L2" s="11" t="inlineStr">
         <is>
           <t>TJLP</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M2" s="11" t="inlineStr">
         <is>
           <t>SELIC</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N2" s="11" t="inlineStr">
         <is>
           <t>CDI</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Situacao</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>Venda</t>
+      <c r="O2" s="11" t="inlineStr">
+        <is>
+          <t>Situação</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="12" t="n">
         <v>46044</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="13" t="n">
         <v>5.2845</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="13" t="n">
         <v>5.3045</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="13" t="n">
         <v>5.3112</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="13" t="n">
         <v>5.3118</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="13" t="n">
         <v>5.3246</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="13" t="n">
         <v>5.5046</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="13" t="n">
         <v>6.2322</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="13" t="n">
         <v>6.2334</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="13" t="n">
         <v>6.7154</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="13" t="n">
         <v>6.7187</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="L3" s="14" t="n"/>
+      <c r="M3" s="14" t="n"/>
+      <c r="N3" s="14" t="n"/>
+      <c r="O3" s="15" t="inlineStr">
         <is>
           <t>OK 22/01/2026 16:43:47</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="16" t="n">
         <v>46045</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="17" t="n">
         <v>5.2895</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="17" t="n">
         <v>5.3095</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="17" t="n">
         <v>5.2872</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="17" t="n">
         <v>5.2879</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="17" t="n">
         <v>5.3183</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="17" t="n">
         <v>5.4983</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="17" t="n">
         <v>6.2162</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="17" t="n">
         <v>6.218</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="17" t="n">
         <v>6.6994</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="17" t="n">
         <v>6.7029</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="L4" s="18" t="n"/>
+      <c r="M4" s="18" t="n"/>
+      <c r="N4" s="18" t="n"/>
+      <c r="O4" s="19" t="inlineStr">
         <is>
           <t>OK 23/01/2026 16:23:25</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="12" t="n">
         <v>46048</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="13" t="n">
         <v>5.2805</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="13" t="n">
         <v>5.3005</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="13" t="n">
         <v>5.2754</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="13" t="n">
         <v>5.276</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="13" t="n">
         <v>5.2984</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="13" t="n">
         <v>5.4784</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="13" t="n">
         <v>6.2746</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="13" t="n">
         <v>6.2763</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="13" t="n">
         <v>6.814</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="13" t="n">
         <v>6.8183</v>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="L5" s="14" t="n"/>
+      <c r="M5" s="14" t="n"/>
+      <c r="N5" s="14" t="n"/>
+      <c r="O5" s="15" t="inlineStr">
         <is>
           <t>OK 26/01/2026 16:10:26</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="16" t="n">
         <v>46057</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="17" t="n">
         <v>5.2303</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="17" t="n">
         <v>5.2503</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="17" t="n">
         <v>5.2353</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="17" t="n">
         <v>5.2359</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="F6" s="18" t="n"/>
+      <c r="G6" s="18" t="n"/>
+      <c r="H6" s="17" t="n">
         <v>6.175</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="17" t="n">
         <v>6.1768</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="17" t="n">
         <v>6.7352</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="17" t="n">
         <v>6.7386</v>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="L6" s="18" t="n"/>
+      <c r="M6" s="18" t="n"/>
+      <c r="N6" s="18" t="n"/>
+      <c r="O6" s="19" t="inlineStr">
         <is>
           <t>OK 04/02/2026 14:31:10</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="12" t="n">
         <v>46064</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="B7" s="14" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="13" t="n">
         <v>5.183</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="13" t="n">
         <v>5.1836</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="F7" s="14" t="n"/>
+      <c r="G7" s="14" t="n"/>
+      <c r="H7" s="13" t="n">
         <v>6.146</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="13" t="n">
         <v>6.1477</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="13" t="n">
         <v>6.7076</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="13" t="n">
         <v>6.7102</v>
       </c>
-      <c r="L7" s="8" t="n">
+      <c r="L7" s="20" t="n">
         <v>0.0919</v>
       </c>
-      <c r="M7" s="8" t="n">
+      <c r="M7" s="20" t="n">
         <v>0.15</v>
       </c>
-      <c r="N7" s="9" t="n">
+      <c r="N7" s="21" t="n">
         <v>0.0551310642</v>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="O7" s="15" t="inlineStr">
         <is>
           <t>OK 11/02/2026 16:53:39</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="16" t="n">
         <v>46065</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="17" t="n">
         <v>5.1836</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="17" t="n">
         <v>5.1856</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="D8" s="18" t="n"/>
+      <c r="E8" s="18" t="n"/>
+      <c r="F8" s="17" t="n">
         <v>5.2147</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="17" t="n">
         <v>5.3947</v>
       </c>
-      <c r="L8" s="8" t="n">
+      <c r="H8" s="18" t="n"/>
+      <c r="I8" s="18" t="n"/>
+      <c r="J8" s="18" t="n"/>
+      <c r="K8" s="18" t="n"/>
+      <c r="L8" s="22" t="n">
         <v>0.0919</v>
       </c>
-      <c r="M8" s="8" t="n">
+      <c r="M8" s="22" t="n">
         <v>0.15</v>
       </c>
-      <c r="N8" s="9" t="n">
+      <c r="N8" s="23" t="n">
         <v>0.0551310642</v>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="O8" s="19" t="inlineStr">
         <is>
           <t>OK 12/02/2026 07:55:30</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:O8"/>
+  <mergeCells count="5">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrigindo erro  na captura do PTAX
</commit_message>
<xml_diff>
--- a/planilhas/cotacoes.xlsx
+++ b/planilhas/cotacoes.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cotacoes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cotacoes'!$A$2:$O$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cotacoes'!$A$2:$O$10</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -17,19 +17,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF1F2937"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -43,12 +54,32 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECF3FB"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,16 +112,49 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF9CB6D9"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF9CB6D9"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF9CB6D9"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF9CB6D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9CB6D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF9CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9CB6D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF9CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9CB6D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9CB6D9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -108,98 +172,88 @@
         <color rgb="009CB6D9"/>
       </bottom>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="009CB6D9"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="009CB6D9"/>
-      </right>
-      <top style="thin">
-        <color rgb="009CB6D9"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="009CB6D9"/>
-      </right>
-      <top style="thin">
-        <color rgb="009CB6D9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="009CB6D9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="10" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,11 +599,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="46.7109375" defaultRowHeight="15"/>
@@ -561,379 +615,473 @@
     <col width="11.5" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="12.5" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="11.5" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="11.5" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="11.5" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="11.5" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="11.5" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="11.5" customWidth="1" min="8" max="11"/>
+    <col width="11.5" customWidth="1" min="9" max="9"/>
+    <col width="11.5" customWidth="1" min="10" max="10"/>
+    <col width="11.5" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="13"/>
     <col width="10" customWidth="1" min="13" max="13"/>
     <col width="12.5" customWidth="1" min="14" max="14"/>
     <col width="30" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
-      <c r="A1" s="10" t="n"/>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="A1" s="14" t="n"/>
+      <c r="B1" s="14" t="inlineStr">
         <is>
           <t>Dólar Oficial 
 (Fechamento)</t>
         </is>
       </c>
-      <c r="C1" s="10" t="n"/>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="C1" s="14" t="n"/>
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Dólar PTAX</t>
         </is>
       </c>
-      <c r="E1" s="10" t="n"/>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="E1" s="14" t="n"/>
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>Dólar Turismo</t>
         </is>
       </c>
-      <c r="G1" s="10" t="n"/>
-      <c r="H1" s="10" t="inlineStr">
+      <c r="G1" s="14" t="n"/>
+      <c r="H1" s="14" t="inlineStr">
         <is>
           <t>Euro PTAX</t>
         </is>
       </c>
-      <c r="I1" s="10" t="n"/>
-      <c r="J1" s="10" t="inlineStr">
+      <c r="I1" s="14" t="n"/>
+      <c r="J1" s="14" t="inlineStr">
         <is>
           <t>CHF PTAX</t>
         </is>
       </c>
-      <c r="K1" s="10" t="n"/>
-      <c r="L1" s="10" t="n"/>
-      <c r="M1" s="10" t="n"/>
-      <c r="N1" s="10" t="n"/>
-      <c r="O1" s="10" t="n"/>
+      <c r="K1" s="14" t="n"/>
+      <c r="L1" s="14" t="n"/>
+      <c r="M1" s="14" t="n"/>
+      <c r="N1" s="14" t="n"/>
+      <c r="O1" s="14" t="n"/>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="11" t="inlineStr">
+      <c r="A2" s="15" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="B2" s="11" t="inlineStr">
+      <c r="B2" s="15" t="inlineStr">
         <is>
           <t>Compra</t>
         </is>
       </c>
-      <c r="C2" s="11" t="inlineStr">
+      <c r="C2" s="15" t="inlineStr">
         <is>
           <t>Venda</t>
         </is>
       </c>
-      <c r="D2" s="11" t="inlineStr">
+      <c r="D2" s="15" t="inlineStr">
         <is>
           <t>Compra</t>
         </is>
       </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="E2" s="15" t="inlineStr">
         <is>
           <t>Venda</t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr">
+      <c r="F2" s="15" t="inlineStr">
         <is>
           <t>Compra</t>
         </is>
       </c>
-      <c r="G2" s="11" t="inlineStr">
+      <c r="G2" s="15" t="inlineStr">
         <is>
           <t>Venda</t>
         </is>
       </c>
-      <c r="H2" s="11" t="inlineStr">
+      <c r="H2" s="15" t="inlineStr">
         <is>
           <t>Compra</t>
         </is>
       </c>
-      <c r="I2" s="11" t="inlineStr">
+      <c r="I2" s="15" t="inlineStr">
         <is>
           <t>Venda</t>
         </is>
       </c>
-      <c r="J2" s="11" t="inlineStr">
+      <c r="J2" s="15" t="inlineStr">
         <is>
           <t>Compra</t>
         </is>
       </c>
-      <c r="K2" s="11" t="inlineStr">
+      <c r="K2" s="15" t="inlineStr">
         <is>
           <t>Venda</t>
         </is>
       </c>
-      <c r="L2" s="11" t="inlineStr">
+      <c r="L2" s="15" t="inlineStr">
         <is>
           <t>TJLP</t>
         </is>
       </c>
-      <c r="M2" s="11" t="inlineStr">
+      <c r="M2" s="15" t="inlineStr">
         <is>
           <t>SELIC</t>
         </is>
       </c>
-      <c r="N2" s="11" t="inlineStr">
+      <c r="N2" s="15" t="inlineStr">
         <is>
           <t>CDI</t>
         </is>
       </c>
-      <c r="O2" s="11" t="inlineStr">
+      <c r="O2" s="15" t="inlineStr">
         <is>
           <t>Situação</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="n">
+      <c r="A3" s="16" t="n">
         <v>46044</v>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="17" t="n">
         <v>5.2845</v>
       </c>
-      <c r="C3" s="13" t="n">
+      <c r="C3" s="17" t="n">
         <v>5.3045</v>
       </c>
-      <c r="D3" s="13" t="n">
+      <c r="D3" s="17" t="n">
         <v>5.3112</v>
       </c>
-      <c r="E3" s="13" t="n">
+      <c r="E3" s="17" t="n">
         <v>5.3118</v>
       </c>
-      <c r="F3" s="13" t="n">
+      <c r="F3" s="17" t="n">
         <v>5.3246</v>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="17" t="n">
         <v>5.5046</v>
       </c>
-      <c r="H3" s="13" t="n">
+      <c r="H3" s="17" t="n">
         <v>6.2322</v>
       </c>
-      <c r="I3" s="13" t="n">
+      <c r="I3" s="17" t="n">
         <v>6.2334</v>
       </c>
-      <c r="J3" s="13" t="n">
+      <c r="J3" s="17" t="n">
         <v>6.7154</v>
       </c>
-      <c r="K3" s="13" t="n">
+      <c r="K3" s="17" t="n">
         <v>6.7187</v>
       </c>
-      <c r="L3" s="14" t="n"/>
-      <c r="M3" s="14" t="n"/>
-      <c r="N3" s="14" t="n"/>
-      <c r="O3" s="15" t="inlineStr">
+      <c r="L3" s="18" t="n"/>
+      <c r="M3" s="18" t="n"/>
+      <c r="N3" s="18" t="n"/>
+      <c r="O3" s="19" t="inlineStr">
         <is>
           <t>OK 22/01/2026 16:43:47</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="20" t="n">
         <v>46045</v>
       </c>
-      <c r="B4" s="17" t="n">
+      <c r="B4" s="21" t="n">
         <v>5.2895</v>
       </c>
-      <c r="C4" s="17" t="n">
+      <c r="C4" s="21" t="n">
         <v>5.3095</v>
       </c>
-      <c r="D4" s="17" t="n">
+      <c r="D4" s="21" t="n">
         <v>5.2872</v>
       </c>
-      <c r="E4" s="17" t="n">
+      <c r="E4" s="21" t="n">
         <v>5.2879</v>
       </c>
-      <c r="F4" s="17" t="n">
+      <c r="F4" s="21" t="n">
         <v>5.3183</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="21" t="n">
         <v>5.4983</v>
       </c>
-      <c r="H4" s="17" t="n">
+      <c r="H4" s="21" t="n">
         <v>6.2162</v>
       </c>
-      <c r="I4" s="17" t="n">
+      <c r="I4" s="21" t="n">
         <v>6.218</v>
       </c>
-      <c r="J4" s="17" t="n">
+      <c r="J4" s="21" t="n">
         <v>6.6994</v>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="21" t="n">
         <v>6.7029</v>
       </c>
-      <c r="L4" s="18" t="n"/>
-      <c r="M4" s="18" t="n"/>
-      <c r="N4" s="18" t="n"/>
-      <c r="O4" s="19" t="inlineStr">
+      <c r="L4" s="22" t="n"/>
+      <c r="M4" s="22" t="n"/>
+      <c r="N4" s="22" t="n"/>
+      <c r="O4" s="23" t="inlineStr">
         <is>
           <t>OK 23/01/2026 16:23:25</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="n">
+      <c r="A5" s="16" t="n">
         <v>46048</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="17" t="n">
         <v>5.2805</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="17" t="n">
         <v>5.3005</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="17" t="n">
         <v>5.2754</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="17" t="n">
         <v>5.276</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="17" t="n">
         <v>5.2984</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="17" t="n">
         <v>5.4784</v>
       </c>
-      <c r="H5" s="13" t="n">
+      <c r="H5" s="17" t="n">
         <v>6.2746</v>
       </c>
-      <c r="I5" s="13" t="n">
+      <c r="I5" s="17" t="n">
         <v>6.2763</v>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J5" s="17" t="n">
         <v>6.814</v>
       </c>
-      <c r="K5" s="13" t="n">
+      <c r="K5" s="17" t="n">
         <v>6.8183</v>
       </c>
-      <c r="L5" s="14" t="n"/>
-      <c r="M5" s="14" t="n"/>
-      <c r="N5" s="14" t="n"/>
-      <c r="O5" s="15" t="inlineStr">
+      <c r="L5" s="18" t="n"/>
+      <c r="M5" s="18" t="n"/>
+      <c r="N5" s="18" t="n"/>
+      <c r="O5" s="19" t="inlineStr">
         <is>
           <t>OK 26/01/2026 16:10:26</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="16" t="n">
+      <c r="A6" s="20" t="n">
         <v>46057</v>
       </c>
-      <c r="B6" s="17" t="n">
-        <v>5.2303</v>
-      </c>
-      <c r="C6" s="17" t="n">
-        <v>5.2503</v>
-      </c>
-      <c r="D6" s="17" t="n">
+      <c r="B6" s="21" t="n"/>
+      <c r="C6" s="21" t="n"/>
+      <c r="D6" s="21" t="n">
         <v>5.2353</v>
       </c>
-      <c r="E6" s="17" t="n">
+      <c r="E6" s="21" t="n">
         <v>5.2359</v>
       </c>
-      <c r="F6" s="18" t="n"/>
-      <c r="G6" s="18" t="n"/>
-      <c r="H6" s="17" t="n">
+      <c r="F6" s="22" t="n"/>
+      <c r="G6" s="22" t="n"/>
+      <c r="H6" s="21" t="n">
         <v>6.175</v>
       </c>
-      <c r="I6" s="17" t="n">
+      <c r="I6" s="21" t="n">
         <v>6.1768</v>
       </c>
-      <c r="J6" s="17" t="n">
+      <c r="J6" s="21" t="n">
         <v>6.7352</v>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="21" t="n">
         <v>6.7386</v>
       </c>
-      <c r="L6" s="18" t="n"/>
-      <c r="M6" s="18" t="n"/>
-      <c r="N6" s="18" t="n"/>
-      <c r="O6" s="19" t="inlineStr">
-        <is>
-          <t>OK 04/02/2026 14:31:10</t>
+      <c r="L6" s="22" t="n"/>
+      <c r="M6" s="22" t="n"/>
+      <c r="N6" s="22" t="n"/>
+      <c r="O6" s="23" t="inlineStr">
+        <is>
+          <t>OK 04/02/2026 16:49:52</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="n">
-        <v>46064</v>
-      </c>
-      <c r="B7" s="14" t="n"/>
-      <c r="C7" s="14" t="n"/>
-      <c r="D7" s="13" t="n">
-        <v>5.183</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <v>5.1836</v>
-      </c>
-      <c r="F7" s="14" t="n"/>
-      <c r="G7" s="14" t="n"/>
-      <c r="H7" s="13" t="n">
-        <v>6.146</v>
-      </c>
-      <c r="I7" s="13" t="n">
-        <v>6.1477</v>
-      </c>
-      <c r="J7" s="13" t="n">
-        <v>6.7076</v>
-      </c>
-      <c r="K7" s="13" t="n">
-        <v>6.7102</v>
-      </c>
-      <c r="L7" s="20" t="n">
-        <v>0.0919</v>
-      </c>
-      <c r="M7" s="20" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="N7" s="21" t="n">
-        <v>0.0551310642</v>
-      </c>
-      <c r="O7" s="15" t="inlineStr">
-        <is>
-          <t>OK 11/02/2026 16:53:39</t>
+      <c r="A7" s="16" t="n">
+        <v>46058</v>
+      </c>
+      <c r="B7" s="17" t="n">
+        <v>5.2395</v>
+      </c>
+      <c r="C7" s="17" t="n">
+        <v>5.2595</v>
+      </c>
+      <c r="D7" s="17" t="n">
+        <v>5.2574</v>
+      </c>
+      <c r="E7" s="17" t="n">
+        <v>5.258</v>
+      </c>
+      <c r="F7" s="17" t="n">
+        <v>5.3124</v>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v>5.4924</v>
+      </c>
+      <c r="H7" s="17" t="n">
+        <v>6.1985</v>
+      </c>
+      <c r="I7" s="17" t="n">
+        <v>6.2002</v>
+      </c>
+      <c r="J7" s="17" t="n">
+        <v>6.7637</v>
+      </c>
+      <c r="K7" s="17" t="n">
+        <v>6.7653</v>
+      </c>
+      <c r="L7" s="18" t="n"/>
+      <c r="M7" s="18" t="n"/>
+      <c r="N7" s="18" t="n"/>
+      <c r="O7" s="19" t="inlineStr">
+        <is>
+          <t>OK 05/02/2026 14:15:29</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="n">
+      <c r="A8" s="20" t="n">
+        <v>46063</v>
+      </c>
+      <c r="B8" s="22" t="n"/>
+      <c r="C8" s="22" t="n"/>
+      <c r="D8" s="21" t="n">
+        <v>5.2015</v>
+      </c>
+      <c r="E8" s="21" t="n">
+        <v>5.2021</v>
+      </c>
+      <c r="F8" s="22" t="n"/>
+      <c r="G8" s="22" t="n"/>
+      <c r="H8" s="21" t="n">
+        <v>6.1965</v>
+      </c>
+      <c r="I8" s="21" t="n">
+        <v>6.1983</v>
+      </c>
+      <c r="J8" s="21" t="n">
+        <v>6.7967</v>
+      </c>
+      <c r="K8" s="21" t="n">
+        <v>6.8001</v>
+      </c>
+      <c r="L8" s="22" t="n"/>
+      <c r="M8" s="22" t="n"/>
+      <c r="N8" s="22" t="n"/>
+      <c r="O8" s="23" t="inlineStr">
+        <is>
+          <t>OK 10/02/2026 17:10:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="16" t="n">
+        <v>46064</v>
+      </c>
+      <c r="B9" s="17" t="n">
+        <v>5.1925</v>
+      </c>
+      <c r="C9" s="17" t="n">
+        <v>5.1945</v>
+      </c>
+      <c r="D9" s="17" t="n">
+        <v>5.183</v>
+      </c>
+      <c r="E9" s="17" t="n">
+        <v>5.1836</v>
+      </c>
+      <c r="F9" s="17" t="n">
+        <v>5.2175</v>
+      </c>
+      <c r="G9" s="17" t="n">
+        <v>5.3975</v>
+      </c>
+      <c r="H9" s="17" t="n">
+        <v>6.146</v>
+      </c>
+      <c r="I9" s="17" t="n">
+        <v>6.1477</v>
+      </c>
+      <c r="J9" s="17" t="n">
+        <v>6.7076</v>
+      </c>
+      <c r="K9" s="17" t="n">
+        <v>6.7102</v>
+      </c>
+      <c r="L9" s="24" t="n">
+        <v>0.0919</v>
+      </c>
+      <c r="M9" s="24" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N9" s="18" t="n">
+        <v>0.0551310642</v>
+      </c>
+      <c r="O9" s="19" t="inlineStr">
+        <is>
+          <t>OK 11/02/2026 13:15:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="25" t="n">
         <v>46065</v>
       </c>
-      <c r="B8" s="17" t="n">
+      <c r="B10" s="21" t="n">
         <v>5.1836</v>
       </c>
-      <c r="C8" s="17" t="n">
+      <c r="C10" s="21" t="n">
         <v>5.1856</v>
       </c>
-      <c r="D8" s="18" t="n"/>
-      <c r="E8" s="18" t="n"/>
-      <c r="F8" s="17" t="n">
+      <c r="D10" s="21" t="n">
+        <v>5.1668</v>
+      </c>
+      <c r="E10" s="21" t="n">
+        <v>5.1674</v>
+      </c>
+      <c r="F10" s="21" t="n">
         <v>5.2147</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G10" s="21" t="n">
         <v>5.3947</v>
       </c>
-      <c r="H8" s="18" t="n"/>
-      <c r="I8" s="18" t="n"/>
-      <c r="J8" s="18" t="n"/>
-      <c r="K8" s="18" t="n"/>
-      <c r="L8" s="22" t="n">
+      <c r="H10" s="21" t="n">
+        <v>6.1407</v>
+      </c>
+      <c r="I10" s="21" t="n">
+        <v>6.1425</v>
+      </c>
+      <c r="J10" s="21" t="n">
+        <v>6.7285</v>
+      </c>
+      <c r="K10" s="21" t="n">
+        <v>6.7319</v>
+      </c>
+      <c r="L10" s="26" t="n">
         <v>0.0919</v>
       </c>
-      <c r="M8" s="22" t="n">
+      <c r="M10" s="26" t="n">
         <v>0.15</v>
       </c>
-      <c r="N8" s="23" t="n">
+      <c r="N10" s="22" t="n">
         <v>0.0551310642</v>
       </c>
-      <c r="O8" s="19" t="inlineStr">
-        <is>
-          <t>OK 12/02/2026 07:55:30</t>
+      <c r="O10" s="23" t="inlineStr">
+        <is>
+          <t>OK 12/02/2026 14:52:54</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O8"/>
+  <autoFilter ref="A2:O10"/>
   <mergeCells count="5">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="H1:I1"/>

</xml_diff>

<commit_message>
corrigindo comportamento de formatacao do formato dos numeros
</commit_message>
<xml_diff>
--- a/planilhas/cotacoes.xlsx
+++ b/planilhas/cotacoes.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Cotacoes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cotacoes'!$A$2:$O$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cotacoes'!$A$2:$O$11</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -17,9 +17,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -102,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -172,11 +174,44 @@
         <color rgb="009CB6D9"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="009CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="009CB6D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="009CB6D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="009CB6D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -254,6 +289,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -599,7 +652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -741,7 +794,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="n">
+      <c r="A3" s="27" t="n">
         <v>46044</v>
       </c>
       <c r="B3" s="17" t="n">
@@ -784,7 +837,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="20" t="n">
+      <c r="A4" s="25" t="n">
         <v>46045</v>
       </c>
       <c r="B4" s="21" t="n">
@@ -827,7 +880,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="16" t="n">
+      <c r="A5" s="27" t="n">
         <v>46048</v>
       </c>
       <c r="B5" s="17" t="n">
@@ -870,7 +923,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="n">
+      <c r="A6" s="25" t="n">
         <v>46057</v>
       </c>
       <c r="B6" s="21" t="n"/>
@@ -905,7 +958,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="n">
+      <c r="A7" s="27" t="n">
         <v>46058</v>
       </c>
       <c r="B7" s="17" t="n">
@@ -948,7 +1001,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="20" t="n">
+      <c r="A8" s="25" t="n">
         <v>46063</v>
       </c>
       <c r="B8" s="22" t="n"/>
@@ -983,7 +1036,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="n">
+      <c r="A9" s="27" t="n">
         <v>46064</v>
       </c>
       <c r="B9" s="17" t="n">
@@ -1022,7 +1075,7 @@
       <c r="M9" s="24" t="n">
         <v>0.15</v>
       </c>
-      <c r="N9" s="18" t="n">
+      <c r="N9" s="31" t="n">
         <v>0.0551310642</v>
       </c>
       <c r="O9" s="19" t="inlineStr">
@@ -1071,17 +1124,54 @@
       <c r="M10" s="26" t="n">
         <v>0.15</v>
       </c>
-      <c r="N10" s="22" t="n">
+      <c r="N10" s="32" t="n">
         <v>0.0551310642</v>
       </c>
       <c r="O10" s="23" t="inlineStr">
         <is>
           <t>OK 12/02/2026 14:52:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="27" t="n">
+        <v>46066</v>
+      </c>
+      <c r="B11" s="17" t="n">
+        <v>5.212</v>
+      </c>
+      <c r="C11" s="17" t="n">
+        <v>5.214</v>
+      </c>
+      <c r="D11" s="18" t="n"/>
+      <c r="E11" s="18" t="n"/>
+      <c r="F11" s="17" t="n">
+        <v>5.2223</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>5.4023</v>
+      </c>
+      <c r="H11" s="18" t="n"/>
+      <c r="I11" s="18" t="n"/>
+      <c r="J11" s="18" t="n"/>
+      <c r="K11" s="18" t="n"/>
+      <c r="L11" s="24" t="n">
+        <v>0.0919</v>
+      </c>
+      <c r="M11" s="24" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N11" s="31" t="n">
+        <v>0.0551310642</v>
+      </c>
+      <c r="O11" s="19" t="inlineStr">
+        <is>
+          <t>OK 13/02/2026 07:27:55</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O10"/>
+  <autoFilter ref="A2:O11"/>
   <mergeCells count="5">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="H1:I1"/>

</xml_diff>